<commit_message>
trying to fix ValueError
</commit_message>
<xml_diff>
--- a/tests_params.xlsx
+++ b/tests_params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uconn\lsh_pse_implem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78D9CC6-7F93-4D9B-922A-18A50B683E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9463B2-BA06-403B-8882-75C28E0362A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B5B036F5-B8FA-4E49-9C02-9188FD27AC5A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="26">
   <si>
     <t>DB size</t>
   </si>
@@ -2406,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3B7726-1647-46AA-8D92-0F4544192CBC}">
   <dimension ref="A6:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3917,9 +3917,9 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D44" s="64"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="10"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -3929,7 +3929,7 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
-      <c r="P44" s="2"/>
+      <c r="P44" s="1"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D45" s="30"/>
@@ -3962,19 +3962,45 @@
       <c r="P46" s="2"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D47" s="30"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="2"/>
+      <c r="D47" s="64">
+        <v>2500</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" s="10">
+        <v>19</v>
+      </c>
+      <c r="G47" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="J47" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="K47" s="1">
+        <v>21.7</v>
+      </c>
+      <c r="L47" s="1">
+        <v>173</v>
+      </c>
+      <c r="M47" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="N47" s="1">
+        <v>14</v>
+      </c>
+      <c r="O47" s="1">
+        <v>27.3</v>
+      </c>
+      <c r="P47" s="2">
+        <v>177</v>
+      </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D48" s="30"/>

</xml_diff>